<commit_message>
make the regression model
</commit_message>
<xml_diff>
--- a/data/house_price.xlsx
+++ b/data/house_price.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\programming folder\computer science and stocks\machine learning\thoery_of_ml\project_one\linearRegression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\programming folder\computer science and stocks\machine learning\thoery_of_ml\project_one\linearRegression\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4624EB94-514E-4F78-86F8-84D24D85B2A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D3DB5B-4138-4965-A20A-979EBF195F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3270" yWindow="2690" windowWidth="14400" windowHeight="7270" xr2:uid="{00B56CFD-A575-4166-BC36-F3DAA51247BC}"/>
   </bookViews>
@@ -385,7 +385,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>